<commit_message>
Versão enviada para Marco Tulio
</commit_message>
<xml_diff>
--- a/data/estatisticas.xlsx
+++ b/data/estatisticas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Projeto</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Valor do batching moving</t>
+  </si>
+  <si>
+    <t>Frequência (batching moving)</t>
   </si>
 </sst>
 </file>
@@ -89,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,20 +182,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:F14"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,6 +442,46 @@
       <c r="F14" s="1" t="n">
         <f aca="false">TRUNC(C14*1.5)</f>
         <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>